<commit_message>
added the web templates
</commit_message>
<xml_diff>
--- a/output/vote_results/vote_results_faster.xlsx
+++ b/output/vote_results/vote_results_faster.xlsx
@@ -476,12 +476,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>image_0018.jpg</t>
+          <t>image_0017.jpg</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>dog</t>
+          <t>invalid_stamp</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -501,11 +501,13 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>invalid symbol or invalid stamp</t>
-        </is>
-      </c>
-      <c r="H2" t="n">
-        <v>237.3010746068453</v>
+          <t>invalid stamp</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>